<commit_message>
Added Fmin constraint to model and case studies
</commit_message>
<xml_diff>
--- a/pareto/case_studies/large_case_study_Li.xlsx
+++ b/pareto/case_studies/large_case_study_Li.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arshb11/main/Grad_Research/CM/project-pareto/pareto/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E35D98E-FEC3-DA4F-8CC3-5433230AFF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B9439B-E25B-2646-8BC7-33EC94360CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" tabRatio="834" firstSheet="52" activeTab="59" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" tabRatio="834" firstSheet="76" activeTab="84" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -97,12 +97,13 @@
     <sheet name="PadWaterQuality" sheetId="99" r:id="rId82"/>
     <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId83"/>
     <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId84"/>
-    <sheet name="MinResidualQuality" sheetId="115" r:id="rId85"/>
-    <sheet name="ComponentPrice" sheetId="116" r:id="rId86"/>
-    <sheet name="ComponentTreatment" sheetId="117" r:id="rId87"/>
+    <sheet name="MinTreatmentFlow" sheetId="126" r:id="rId85"/>
+    <sheet name="MinResidualQuality" sheetId="115" r:id="rId86"/>
+    <sheet name="ComponentPrice" sheetId="116" r:id="rId87"/>
+    <sheet name="ComponentTreatment" sheetId="117" r:id="rId88"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId88"/>
+    <externalReference r:id="rId89"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="70" hidden="1">#REF!</definedName>
@@ -129,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3302" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3309" uniqueCount="310">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1057,6 +1058,9 @@
   <si>
     <t>List of all Water Quality Components [-]</t>
   </si>
+  <si>
+    <t>Minimum inlet flow required at each treatment site</t>
+  </si>
 </sst>
 </file>
 
@@ -1657,7 +1661,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1972,7 +1976,6 @@
     <xf numFmtId="11" fontId="9" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -31053,7 +31056,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -39771,7 +39774,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40536,6 +40539,69 @@
 </file>
 
 <file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC4A4C6-1F13-8F40-81F5-594539BEBFCA}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="34">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F899846-250B-DB4B-8A11-709217E17428}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -40598,7 +40664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64AF8D8-BCEF-F245-8739-3BFAA192AA47}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -40661,7 +40727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E02D577-3E8C-444E-87B2-8DF0DDD275D2}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -40745,7 +40811,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="130"/>
+      <c r="A3" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor changes to jupyter notebook and case studies
</commit_message>
<xml_diff>
--- a/pareto/case_studies/large_case_study_Li.xlsx
+++ b/pareto/case_studies/large_case_study_Li.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arshb11/main/Grad_Research/CM/project-pareto/pareto/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FBA36D-0757-0442-862D-0C0C2ACC7724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98797434-9313-C348-ABDA-34D85CDFBBDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" tabRatio="834" activeTab="1" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17620" tabRatio="834" firstSheet="51" activeTab="60" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="230">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -761,12 +761,6 @@
     <t>Li</t>
   </si>
   <si>
-    <t>Minimum Water Quality out of Residual Stream</t>
-  </si>
-  <si>
-    <t>Price earned based on each residuual treatment node [USD/mg]</t>
-  </si>
-  <si>
     <t>Choice on whether the site will treat that componenet or not</t>
   </si>
   <si>
@@ -782,7 +776,19 @@
     <t>List of all Water Quality Components [-]</t>
   </si>
   <si>
-    <t>Minimum inlet flow required at each treatment site</t>
+    <t>Price earned based on each residuual treatment node [USD/bbl]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum Water Quality out of Residual Stream </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum inlet flow required at each treatment site </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table of Initial Storage Water Quality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table of production pad water quality </t>
   </si>
 </sst>
 </file>
@@ -6060,7 +6066,7 @@
   </sheetPr>
   <dimension ref="C3:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12262,7 +12268,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="75" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B1" s="75"/>
     </row>
@@ -28212,7 +28218,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -28267,7 +28273,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -29398,7 +29404,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29412,9 +29418,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -29575,7 +29580,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29584,9 +29589,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="e">
-        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [",VLOOKUP("concentration",#REF!, 2, FALSE),"]")</f>
-        <v>#REF!</v>
+      <c r="A1" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -29635,7 +29639,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29695,7 +29699,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29705,7 +29709,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -29817,7 +29821,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29827,7 +29831,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -29879,7 +29883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E02D577-3E8C-444E-87B2-8DF0DDD275D2}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -29887,7 +29891,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -29999,7 +30003,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="16" x14ac:dyDescent="0.2">

</xml_diff>